<commit_message>
Updated Geocode and add more refference for home
- Geocode now is working fine
- added refference for Carousel, just have to figure how to setOnclick based on image

TODO : Fix the onclicklistener on image
</commit_message>
<xml_diff>
--- a/Objek/Mapping.xlsx
+++ b/Objek/Mapping.xlsx
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:DC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U14" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="BW20" sqref="BW20"/>
+    <sheetView tabSelected="1" topLeftCell="BY19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CF2" sqref="CF2:CL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +652,12 @@
       <c r="CD2" s="25"/>
       <c r="CE2" s="25"/>
       <c r="CF2" s="25"/>
+      <c r="CG2" s="24"/>
+      <c r="CH2" s="24"/>
+      <c r="CI2" s="24"/>
+      <c r="CJ2" s="24"/>
+      <c r="CK2" s="24"/>
+      <c r="CL2" s="24"/>
       <c r="CM2" s="17" t="s">
         <v>0</v>
       </c>
@@ -748,6 +754,12 @@
       <c r="CD3" s="25"/>
       <c r="CE3" s="25"/>
       <c r="CF3" s="25"/>
+      <c r="CG3" s="24"/>
+      <c r="CH3" s="24"/>
+      <c r="CI3" s="24"/>
+      <c r="CJ3" s="24"/>
+      <c r="CK3" s="24"/>
+      <c r="CL3" s="24"/>
       <c r="CM3" s="17" t="s">
         <v>0</v>
       </c>
@@ -844,6 +856,12 @@
       <c r="CD4" s="25"/>
       <c r="CE4" s="25"/>
       <c r="CF4" s="25"/>
+      <c r="CG4" s="24"/>
+      <c r="CH4" s="24"/>
+      <c r="CI4" s="24"/>
+      <c r="CJ4" s="24"/>
+      <c r="CK4" s="24"/>
+      <c r="CL4" s="24"/>
       <c r="CM4" s="17" t="s">
         <v>0</v>
       </c>
@@ -940,6 +958,12 @@
       <c r="CD5" s="25"/>
       <c r="CE5" s="25"/>
       <c r="CF5" s="25"/>
+      <c r="CG5" s="24"/>
+      <c r="CH5" s="24"/>
+      <c r="CI5" s="24"/>
+      <c r="CJ5" s="24"/>
+      <c r="CK5" s="24"/>
+      <c r="CL5" s="24"/>
       <c r="CM5" s="17" t="s">
         <v>0</v>
       </c>
@@ -1036,6 +1060,12 @@
       <c r="CD6" s="25"/>
       <c r="CE6" s="25"/>
       <c r="CF6" s="25"/>
+      <c r="CG6" s="24"/>
+      <c r="CH6" s="24"/>
+      <c r="CI6" s="24"/>
+      <c r="CJ6" s="24"/>
+      <c r="CK6" s="24"/>
+      <c r="CL6" s="24"/>
       <c r="CM6" s="17" t="s">
         <v>0</v>
       </c>
@@ -1132,6 +1162,12 @@
       <c r="CD7" s="25"/>
       <c r="CE7" s="25"/>
       <c r="CF7" s="25"/>
+      <c r="CG7" s="24"/>
+      <c r="CH7" s="24"/>
+      <c r="CI7" s="24"/>
+      <c r="CJ7" s="24"/>
+      <c r="CK7" s="24"/>
+      <c r="CL7" s="24"/>
       <c r="CM7" s="17" t="s">
         <v>0</v>
       </c>
@@ -1228,6 +1264,12 @@
       <c r="CD8" s="25"/>
       <c r="CE8" s="25"/>
       <c r="CF8" s="25"/>
+      <c r="CG8" s="24"/>
+      <c r="CH8" s="24"/>
+      <c r="CI8" s="24"/>
+      <c r="CJ8" s="24"/>
+      <c r="CK8" s="24"/>
+      <c r="CL8" s="24"/>
       <c r="CM8" s="17" t="s">
         <v>0</v>
       </c>
@@ -1324,6 +1366,12 @@
       <c r="CD9" s="25"/>
       <c r="CE9" s="25"/>
       <c r="CF9" s="25"/>
+      <c r="CG9" s="24"/>
+      <c r="CH9" s="24"/>
+      <c r="CI9" s="24"/>
+      <c r="CJ9" s="24"/>
+      <c r="CK9" s="24"/>
+      <c r="CL9" s="24"/>
       <c r="CM9" s="17" t="s">
         <v>0</v>
       </c>
@@ -1420,6 +1468,12 @@
       <c r="CD10" s="25"/>
       <c r="CE10" s="25"/>
       <c r="CF10" s="25"/>
+      <c r="CG10" s="24"/>
+      <c r="CH10" s="24"/>
+      <c r="CI10" s="24"/>
+      <c r="CJ10" s="24"/>
+      <c r="CK10" s="24"/>
+      <c r="CL10" s="24"/>
       <c r="CM10" s="17" t="s">
         <v>0</v>
       </c>
@@ -1516,6 +1570,12 @@
       <c r="CD11" s="25"/>
       <c r="CE11" s="25"/>
       <c r="CF11" s="25"/>
+      <c r="CG11" s="24"/>
+      <c r="CH11" s="24"/>
+      <c r="CI11" s="24"/>
+      <c r="CJ11" s="24"/>
+      <c r="CK11" s="24"/>
+      <c r="CL11" s="24"/>
       <c r="CM11" s="17" t="s">
         <v>0</v>
       </c>
@@ -1612,6 +1672,12 @@
       <c r="CD12" s="25"/>
       <c r="CE12" s="25"/>
       <c r="CF12" s="25"/>
+      <c r="CG12" s="24"/>
+      <c r="CH12" s="24"/>
+      <c r="CI12" s="24"/>
+      <c r="CJ12" s="24"/>
+      <c r="CK12" s="24"/>
+      <c r="CL12" s="24"/>
       <c r="CM12" s="17" t="s">
         <v>0</v>
       </c>
@@ -1708,6 +1774,12 @@
       <c r="CD13" s="25"/>
       <c r="CE13" s="25"/>
       <c r="CF13" s="25"/>
+      <c r="CG13" s="24"/>
+      <c r="CH13" s="24"/>
+      <c r="CI13" s="24"/>
+      <c r="CJ13" s="24"/>
+      <c r="CK13" s="24"/>
+      <c r="CL13" s="24"/>
       <c r="CM13" s="17" t="s">
         <v>0</v>
       </c>
@@ -1804,6 +1876,12 @@
       <c r="CD14" s="25"/>
       <c r="CE14" s="25"/>
       <c r="CF14" s="25"/>
+      <c r="CG14" s="24"/>
+      <c r="CH14" s="24"/>
+      <c r="CI14" s="24"/>
+      <c r="CJ14" s="24"/>
+      <c r="CK14" s="24"/>
+      <c r="CL14" s="24"/>
       <c r="CM14" s="17" t="s">
         <v>0</v>
       </c>
@@ -1900,6 +1978,12 @@
       <c r="CD15" s="25"/>
       <c r="CE15" s="25"/>
       <c r="CF15" s="25"/>
+      <c r="CG15" s="24"/>
+      <c r="CH15" s="24"/>
+      <c r="CI15" s="24"/>
+      <c r="CJ15" s="24"/>
+      <c r="CK15" s="24"/>
+      <c r="CL15" s="24"/>
       <c r="CM15" s="17" t="s">
         <v>0</v>
       </c>

</xml_diff>